<commit_message>
added example/placeholder normunit / building areas for Com
</commit_message>
<xml_diff>
--- a/scripts/data transformation/Normunits.xlsx
+++ b/scripts/data transformation/Normunits.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hou7002\Projects\CPUC_DEER\EnergyPlus Transition\Task 2\Modelkit_Results_Standardized\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylian\Documents\DEER_prototypes_Dec2023\DEER-Prototypes-EnergyPlus\scripts\data transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAABF811-914B-4B3B-914C-372EF019EE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7251F448-0D27-4730-BD52-0F8BA2EB8BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
+    <workbookView xWindow="-26835" yWindow="510" windowWidth="21645" windowHeight="11475" activeTab="3" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
   </bookViews>
   <sheets>
     <sheet name="DMo" sheetId="1" r:id="rId1"/>
     <sheet name="MFm" sheetId="2" r:id="rId2"/>
     <sheet name="SFm" sheetId="3" r:id="rId3"/>
+    <sheet name="Com" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="56">
   <si>
     <t>Normunit</t>
   </si>
@@ -138,6 +139,72 @@
   </si>
   <si>
     <t>Refrigerator/Freezer</t>
+  </si>
+  <si>
+    <t>BldgLoc</t>
+  </si>
+  <si>
+    <t>BldgType</t>
+  </si>
+  <si>
+    <t>Asm</t>
+  </si>
+  <si>
+    <t>ECC</t>
+  </si>
+  <si>
+    <t>EPr</t>
+  </si>
+  <si>
+    <t>ERC</t>
+  </si>
+  <si>
+    <t>ESe</t>
+  </si>
+  <si>
+    <t>EUn</t>
+  </si>
+  <si>
+    <t>Hsp</t>
+  </si>
+  <si>
+    <t>Htl</t>
+  </si>
+  <si>
+    <t>MBT</t>
+  </si>
+  <si>
+    <t>MLI</t>
+  </si>
+  <si>
+    <t>Mtl</t>
+  </si>
+  <si>
+    <t>Nrs</t>
+  </si>
+  <si>
+    <t>OfL</t>
+  </si>
+  <si>
+    <t>OfS</t>
+  </si>
+  <si>
+    <t>RFF</t>
+  </si>
+  <si>
+    <t>RSD</t>
+  </si>
+  <si>
+    <t>Rt3</t>
+  </si>
+  <si>
+    <t>RtL</t>
+  </si>
+  <si>
+    <t>RtS</t>
+  </si>
+  <si>
+    <t>SCn</t>
   </si>
 </sst>
 </file>
@@ -498,7 +565,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,7 +1286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D254DEF8-D70B-44A9-90B7-19C720405132}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
@@ -2448,4 +2515,259 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F653D6A-2407-4550-AC1C-A4556A4DAC9A}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>100002.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>299999.59999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>50000.14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1920.0170000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>149998.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>930201.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>235501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>139998.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>199999.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>100001.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>30000.07</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>60654.58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>174998.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>10000.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2500.0529999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>5599.9570000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>120000.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>129997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>7999.9290000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>250000.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adjust commercial postprocessing to include Gro prototype
Co-Authored-By: Debrudra20 <126912406+debrudra20@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/scripts/data transformation/Normunits.xlsx
+++ b/scripts/data transformation/Normunits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylian\Documents\DEER_prototypes_Dec2023\DEER-Prototypes-EnergyPlus\scripts\data transformation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DEER-Prototypes-EnergyPlus-TRC_HVAC\scripts\data transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7251F448-0D27-4730-BD52-0F8BA2EB8BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814937CE-3664-44A5-A4D8-2934D4AE77AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26835" yWindow="510" windowWidth="21645" windowHeight="11475" activeTab="3" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
+    <workbookView xWindow="11712" yWindow="-17424" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
   </bookViews>
   <sheets>
     <sheet name="DMo" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="57">
   <si>
     <t>Normunit</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>SCn</t>
+  </si>
+  <si>
+    <t>Gro</t>
   </si>
 </sst>
 </file>
@@ -2519,10 +2522,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F653D6A-2407-4550-AC1C-A4556A4DAC9A}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2615,155 +2618,166 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>235501</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>139998.9</v>
+        <v>235501</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>199999.2</v>
+        <v>139998.9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>100001.1</v>
+        <v>199999.2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>30000.07</v>
+        <v>100001.1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>60654.58</v>
+        <v>30000.07</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>174998.9</v>
+        <v>60654.58</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>10000.08</v>
+        <v>174998.9</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>2500.0529999999999</v>
+        <v>10000.08</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>5599.9570000000003</v>
+        <v>2500.0529999999999</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>120000.5</v>
+        <v>5599.9570000000003</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>129997</v>
+        <v>120000.5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>7999.9290000000001</v>
+        <v>129997</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>7999.9290000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>55</v>
       </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21">
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <v>250000.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Cap-ton capacities for normalizing units
</commit_message>
<xml_diff>
--- a/scripts/data transformation/Normunits.xlsx
+++ b/scripts/data transformation/Normunits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylian\Documents\DEER_prototypes_Dec2023\DEER-Prototypes-EnergyPlus\scripts\data transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7251F448-0D27-4730-BD52-0F8BA2EB8BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE187DA9-F35E-4CDF-9C11-0EF1AE2AB7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26835" yWindow="510" windowWidth="21645" windowHeight="11475" activeTab="3" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
+    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
   </bookViews>
   <sheets>
     <sheet name="DMo" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="59">
   <si>
     <t>Normunit</t>
   </si>
@@ -205,12 +205,24 @@
   </si>
   <si>
     <t>SCn</t>
+  </si>
+  <si>
+    <t>Using sizing capacity from pre-existing base prototype</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>SEER Rated AC/HP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,8 +258,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,18 +575,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2593147D-FBCE-4A43-B94C-18CB04EC4F0B}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -586,8 +600,11 @@
       <c r="D1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -598,7 +615,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -612,7 +629,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -626,7 +643,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -639,6 +656,23 @@
       </c>
       <c r="D5" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>3.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -649,10 +683,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9AEBA2-4873-4E93-88D1-6559970F8CAA}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,7 +695,7 @@
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -677,8 +711,11 @@
       <c r="E1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -689,7 +726,7 @@
         <v>24580</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -703,7 +740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -717,7 +754,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -734,7 +771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -751,7 +788,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -768,7 +805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -785,7 +822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -802,7 +839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -819,7 +856,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -836,7 +873,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -853,7 +890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -870,7 +907,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -887,7 +924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -904,7 +941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1193,7 +1230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -1210,7 +1247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -1227,7 +1264,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1244,7 +1281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -1261,7 +1298,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1274,6 +1311,278 @@
       </c>
       <c r="D37" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+      <c r="F44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+      <c r="F46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="1">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="1">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
+      <c r="F48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="1">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="1">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>58</v>
+      </c>
+      <c r="F51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="1">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="F52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="1">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>58</v>
+      </c>
+      <c r="F53" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1284,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D254DEF8-D70B-44A9-90B7-19C720405132}">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84:D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1296,7 +1605,7 @@
     <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1312,8 +1621,11 @@
       <c r="E1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1324,7 +1636,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1335,7 +1647,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1346,7 +1658,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1357,7 +1669,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1368,7 +1680,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1379,7 +1691,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1390,7 +1702,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1401,7 +1713,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1412,7 +1724,7 @@
         <v>3850</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1423,7 +1735,7 @@
         <v>4140</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1434,7 +1746,7 @@
         <v>3570</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1445,7 +1757,7 @@
         <v>3570</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1456,7 +1768,7 @@
         <v>3570</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1467,7 +1779,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2464,7 +2776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>23</v>
       </c>
@@ -2481,7 +2793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>30</v>
       </c>
@@ -2495,7 +2807,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>32</v>
       </c>
@@ -2508,6 +2820,278 @@
       </c>
       <c r="D83" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="1">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>58</v>
+      </c>
+      <c r="F84" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="1">
+        <v>4</v>
+      </c>
+      <c r="D85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F85" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="1">
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>58</v>
+      </c>
+      <c r="F86" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" s="1">
+        <v>4</v>
+      </c>
+      <c r="D87" t="s">
+        <v>58</v>
+      </c>
+      <c r="F87" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>23</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" s="1">
+        <v>4</v>
+      </c>
+      <c r="D88" t="s">
+        <v>58</v>
+      </c>
+      <c r="F88" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>23</v>
+      </c>
+      <c r="B89" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" s="1">
+        <v>4</v>
+      </c>
+      <c r="D89" t="s">
+        <v>58</v>
+      </c>
+      <c r="F89" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90" s="1">
+        <v>4</v>
+      </c>
+      <c r="D90" t="s">
+        <v>58</v>
+      </c>
+      <c r="F90" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" s="1">
+        <v>4</v>
+      </c>
+      <c r="D91" t="s">
+        <v>58</v>
+      </c>
+      <c r="F91" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" t="s">
+        <v>13</v>
+      </c>
+      <c r="C92" s="1">
+        <v>4</v>
+      </c>
+      <c r="D92" t="s">
+        <v>58</v>
+      </c>
+      <c r="F92" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="1">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>58</v>
+      </c>
+      <c r="F93" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" s="1">
+        <v>5</v>
+      </c>
+      <c r="D94" t="s">
+        <v>58</v>
+      </c>
+      <c r="F94" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>23</v>
+      </c>
+      <c r="B95" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="1">
+        <v>5</v>
+      </c>
+      <c r="D95" t="s">
+        <v>58</v>
+      </c>
+      <c r="F95" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" t="s">
+        <v>17</v>
+      </c>
+      <c r="C96" s="1">
+        <v>5</v>
+      </c>
+      <c r="D96" t="s">
+        <v>58</v>
+      </c>
+      <c r="F96" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>23</v>
+      </c>
+      <c r="B97" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" s="1">
+        <v>5</v>
+      </c>
+      <c r="D97" t="s">
+        <v>58</v>
+      </c>
+      <c r="F97" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>23</v>
+      </c>
+      <c r="B98" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" s="1">
+        <v>5</v>
+      </c>
+      <c r="D98" t="s">
+        <v>58</v>
+      </c>
+      <c r="F98" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>23</v>
+      </c>
+      <c r="B99" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" s="1">
+        <v>5</v>
+      </c>
+      <c r="D99" t="s">
+        <v>58</v>
+      </c>
+      <c r="F99" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2521,7 +3105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F653D6A-2407-4550-AC1C-A4556A4DAC9A}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed commercial normalizing units to cover all bldgtypes
temporary fix. another update with parsing correct cooling capacities coming soon.
</commit_message>
<xml_diff>
--- a/scripts/data transformation/Normunits.xlsx
+++ b/scripts/data transformation/Normunits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DEER-Prototypes-EnergyPlus-TRC_HVAC\scripts\data transformation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylian\Documents\DEER_prototypes_Dec2023\DEER-Prototypes-EnergyPlus\scripts\data transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814937CE-3664-44A5-A4D8-2934D4AE77AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CC5A13-2C42-4765-98FD-EDFD4414960D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11712" yWindow="-17424" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
+    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" activeTab="3" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
   </bookViews>
   <sheets>
     <sheet name="DMo" sheetId="1" r:id="rId1"/>
@@ -36,8 +36,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={762890B7-C641-45A1-9887-23288871FE77}</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{762890B7-C641-45A1-9887-23288871FE77}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Comes from modelkit query.txt lookup</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="69">
   <si>
     <t>Normunit</t>
   </si>
@@ -207,13 +225,52 @@
     <t>SCn</t>
   </si>
   <si>
+    <t>Using sizing capacity from pre-existing base prototype</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>SEER Rated AC/HP</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
     <t>Gro</t>
+  </si>
+  <si>
+    <t>Lib</t>
+  </si>
+  <si>
+    <t>Rel</t>
+  </si>
+  <si>
+    <t>SUn</t>
+  </si>
+  <si>
+    <t>WRf</t>
+  </si>
+  <si>
+    <t>total_area_m2</t>
+  </si>
+  <si>
+    <t>conditioned_area_m2</t>
+  </si>
+  <si>
+    <t>area value in ft2</t>
+  </si>
+  <si>
+    <t>conditioned area is 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -249,8 +306,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -268,10 +327,16 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Liang, Yitian" id="{ACBBF0B3-AFC0-40F5-83A9-0F59F73CE8A1}" userId="S::Yitian.Liang@dnv.com::15f8f0b4-7a89-4cbc-a07d-f4d4b8e31b5d" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -309,7 +374,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -415,7 +480,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -557,26 +622,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2024-05-31T00:05:20.07" personId="{ACBBF0B3-AFC0-40F5-83A9-0F59F73CE8A1}" id="{762890B7-C641-45A1-9887-23288871FE77}">
+    <text>Comes from modelkit query.txt lookup</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2593147D-FBCE-4A43-B94C-18CB04EC4F0B}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,8 +663,11 @@
       <c r="D1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -601,7 +678,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -615,7 +692,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -629,7 +706,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -642,6 +719,23 @@
       </c>
       <c r="D5" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>3.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -652,10 +746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9AEBA2-4873-4E93-88D1-6559970F8CAA}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,7 +758,7 @@
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,8 +774,11 @@
       <c r="E1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -692,7 +789,7 @@
         <v>24580</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -706,7 +803,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -720,7 +817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -737,7 +834,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -754,7 +851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -771,7 +868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -788,7 +885,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -805,7 +902,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -822,7 +919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -839,7 +936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -856,7 +953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -873,7 +970,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -890,7 +987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -907,7 +1004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1196,7 +1293,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -1213,7 +1310,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -1230,7 +1327,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1247,7 +1344,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -1264,7 +1361,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1277,6 +1374,278 @@
       </c>
       <c r="D37" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+      <c r="F44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+      <c r="F46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="1">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="1">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
+      <c r="F48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="1">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="1">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>58</v>
+      </c>
+      <c r="F51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="1">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="F52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="1">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>58</v>
+      </c>
+      <c r="F53" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1287,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D254DEF8-D70B-44A9-90B7-19C720405132}">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84:D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1299,7 +1668,7 @@
     <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1315,8 +1684,11 @@
       <c r="E1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1327,7 +1699,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1338,7 +1710,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1349,7 +1721,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1360,7 +1732,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1371,7 +1743,7 @@
         <v>4320</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1382,7 +1754,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1393,7 +1765,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1404,7 +1776,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1415,7 +1787,7 @@
         <v>3850</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1426,7 +1798,7 @@
         <v>4140</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1437,7 +1809,7 @@
         <v>3570</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1448,7 +1820,7 @@
         <v>3570</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1459,7 +1831,7 @@
         <v>3570</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1470,7 +1842,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2467,7 +2839,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>23</v>
       </c>
@@ -2484,7 +2856,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>30</v>
       </c>
@@ -2498,7 +2870,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>32</v>
       </c>
@@ -2511,6 +2883,278 @@
       </c>
       <c r="D83" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="1">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>58</v>
+      </c>
+      <c r="F84" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="1">
+        <v>4</v>
+      </c>
+      <c r="D85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F85" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="1">
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>58</v>
+      </c>
+      <c r="F86" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" s="1">
+        <v>4</v>
+      </c>
+      <c r="D87" t="s">
+        <v>58</v>
+      </c>
+      <c r="F87" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>23</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" s="1">
+        <v>4</v>
+      </c>
+      <c r="D88" t="s">
+        <v>58</v>
+      </c>
+      <c r="F88" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>23</v>
+      </c>
+      <c r="B89" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" s="1">
+        <v>4</v>
+      </c>
+      <c r="D89" t="s">
+        <v>58</v>
+      </c>
+      <c r="F89" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90" s="1">
+        <v>4</v>
+      </c>
+      <c r="D90" t="s">
+        <v>58</v>
+      </c>
+      <c r="F90" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" s="1">
+        <v>4</v>
+      </c>
+      <c r="D91" t="s">
+        <v>58</v>
+      </c>
+      <c r="F91" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" t="s">
+        <v>13</v>
+      </c>
+      <c r="C92" s="1">
+        <v>4</v>
+      </c>
+      <c r="D92" t="s">
+        <v>58</v>
+      </c>
+      <c r="F92" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="1">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>58</v>
+      </c>
+      <c r="F93" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" s="1">
+        <v>5</v>
+      </c>
+      <c r="D94" t="s">
+        <v>58</v>
+      </c>
+      <c r="F94" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>23</v>
+      </c>
+      <c r="B95" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="1">
+        <v>5</v>
+      </c>
+      <c r="D95" t="s">
+        <v>58</v>
+      </c>
+      <c r="F95" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" t="s">
+        <v>17</v>
+      </c>
+      <c r="C96" s="1">
+        <v>5</v>
+      </c>
+      <c r="D96" t="s">
+        <v>58</v>
+      </c>
+      <c r="F96" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>23</v>
+      </c>
+      <c r="B97" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" s="1">
+        <v>5</v>
+      </c>
+      <c r="D97" t="s">
+        <v>58</v>
+      </c>
+      <c r="F97" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>23</v>
+      </c>
+      <c r="B98" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" s="1">
+        <v>5</v>
+      </c>
+      <c r="D98" t="s">
+        <v>58</v>
+      </c>
+      <c r="F98" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>23</v>
+      </c>
+      <c r="B99" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" s="1">
+        <v>5</v>
+      </c>
+      <c r="D99" t="s">
+        <v>58</v>
+      </c>
+      <c r="F99" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2521,19 +3165,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F653D6A-2407-4550-AC1C-A4556A4DAC9A}">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F653D6A-2407-4550-AC1C-A4556A4DAC9A}">
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F2" sqref="F2:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -2544,13 +3192,22 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -2558,10 +3215,17 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>100002.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6318.03</v>
+      </c>
+      <c r="F2" s="2">
+        <f>D2*10.7639104</f>
+        <v>68006.708824511996</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2569,10 +3233,14 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>299999.59999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>26402.36</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F27" si="0">D3*10.7639104</f>
+        <v>284192.63738854404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2580,10 +3248,14 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>50000.14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3785.38</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>40745.491149952002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -2591,10 +3263,14 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1920.0170000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>267.89</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>2883.5439570559997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -2602,10 +3278,14 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>149998.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6912.2</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>74402.301466880002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -2613,175 +3293,318 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>930201.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>79690.97</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>857786.46076908801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>334.45</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>3599.9898332799999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>4644.87</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>49996.964499647998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>235501</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>45899.29</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>494055.84498361603</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>139998.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>12738.56</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>137116.71846502399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>929.03</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>9999.9956789120006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>199999.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>37156.35</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>399947.62219104002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>100001.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>9291.61</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>100014.057511744</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>30000.07</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2785.81</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>29986.209231424</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>60654.58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>10312.120000000001</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>110998.73571404802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>48</v>
       </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>174998.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>32508.63</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>349919.98054675205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>10000.08</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1858.49</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>20004.619839296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1858.04</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>19999.776079616</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>2500.0529999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>371.26</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>3996.2093751040002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>5599.9570000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1040.99</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="0"/>
+        <v>11205.123087296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>120000.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>22296.73</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>240000.003932992</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>53</v>
       </c>
-      <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>129997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>12123.99</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="0"/>
+        <v>130501.54205049601</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>54</v>
       </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>7999.9290000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1486.69</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>16002.597952576001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>55</v>
       </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>250000.3</v>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>46450.63</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>499990.41934355197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>46450.63</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="0"/>
+        <v>499990.41934355197</v>
+      </c>
+      <c r="H26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>46450.63</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="0"/>
+        <v>499990.41934355197</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to Com.py to accommodate normunit Each
Per PR#56
</commit_message>
<xml_diff>
--- a/scripts/data transformation/Normunits.xlsx
+++ b/scripts/data transformation/Normunits.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylian\Documents\DEER_prototypes_Dec2023\DEER-Prototypes-EnergyPlus\scripts\data transformation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylian\Desktop\postprocessing demo\PR56_review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CC5A13-2C42-4765-98FD-EDFD4414960D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EC7B69-1D83-4854-8A55-90DB85ECE0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" activeTab="3" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="71">
   <si>
     <t>Normunit</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>conditioned area is 0</t>
+  </si>
+  <si>
+    <t>Each</t>
+  </si>
+  <si>
+    <t>added 7/18/2024 to accommodate Normunit = Each</t>
   </si>
 </sst>
 </file>
@@ -3166,10 +3172,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F653D6A-2407-4550-AC1C-A4556A4DAC9A}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F27"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3603,6 +3609,20 @@
         <v>499990.41934355197</v>
       </c>
     </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Com.py to support Cap-Tons normunit
alongside updated Normunits.xlsx (normalizing unit lookup table for all static units other than Cap-Tons)
</commit_message>
<xml_diff>
--- a/scripts/data transformation/Normunits.xlsx
+++ b/scripts/data transformation/Normunits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylian\Documents\DEER_prototypes_Dec2023\DEER-Prototypes-EnergyPlus\scripts\data transformation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylian\Desktop\postprocessing demo\normunit_model_extraction\branch_pp_update_cap_pull\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CC5A13-2C42-4765-98FD-EDFD4414960D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E3B3CC-BEB6-455D-BD10-AB0454329554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" activeTab="3" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
+    <workbookView xWindow="-27684" yWindow="1116" windowWidth="21600" windowHeight="11400" activeTab="3" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
   </bookViews>
   <sheets>
     <sheet name="DMo" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="72">
   <si>
     <t>Normunit</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>conditioned area is 0</t>
+  </si>
+  <si>
+    <t>Each</t>
+  </si>
+  <si>
+    <t>added 7/18/2024 to accommodate Normunit = Each</t>
+  </si>
+  <si>
+    <t>normunit</t>
   </si>
 </sst>
 </file>
@@ -3166,10 +3175,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F653D6A-2407-4550-AC1C-A4556A4DAC9A}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F27"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3189,7 +3198,7 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
         <v>65</v>
@@ -3601,6 +3610,20 @@
       <c r="F27" s="2">
         <f t="shared" si="0"/>
         <v>499990.41934355197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated normunits table + DMo script update
Updated DMo CEDARS 8760 output and relevant tables
</commit_message>
<xml_diff>
--- a/scripts/data transformation/Normunits.xlsx
+++ b/scripts/data transformation/Normunits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylian\Desktop\postprocessing demo\PR56_review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YLIAN\Documents\DEER_github_2025\DEER-Prototypes-EnergyPlus\scripts\data transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EC7B69-1D83-4854-8A55-90DB85ECE0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DE9E93-1157-46D4-A64D-6D4477D55686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" activeTab="3" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
   </bookViews>
   <sheets>
     <sheet name="DMo" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="74">
   <si>
     <t>Normunit</t>
   </si>
@@ -268,6 +268,15 @@
   </si>
   <si>
     <t>added 7/18/2024 to accommodate Normunit = Each</t>
+  </si>
+  <si>
+    <t>Cap-Ton</t>
+  </si>
+  <si>
+    <t>Com Cap-Ton units for SEER rated AC measures from each com bldg type pre prototype</t>
+  </si>
+  <si>
+    <t>Com Cap-Ton units for SEER rated AC measures from each com bldg type pre prototype need to be updated</t>
   </si>
 </sst>
 </file>
@@ -292,12 +301,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -312,10 +327,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2593147D-FBCE-4A43-B94C-18CB04EC4F0B}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9AEBA2-4873-4E93-88D1-6559970F8CAA}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38:D53"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1664,7 +1680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D254DEF8-D70B-44A9-90B7-19C720405132}">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="D84" sqref="D84:D99"/>
     </sheetView>
   </sheetViews>
@@ -3172,22 +3188,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F653D6A-2407-4550-AC1C-A4556A4DAC9A}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32:I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="7" width="11.21875" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -3207,13 +3223,16 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3227,11 +3246,12 @@
         <f>D2*10.7639104</f>
         <v>68006.708824511996</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -3245,8 +3265,9 @@
         <f t="shared" ref="F3:F27" si="0">D3*10.7639104</f>
         <v>284192.63738854404</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3260,8 +3281,9 @@
         <f t="shared" si="0"/>
         <v>40745.491149952002</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -3275,8 +3297,9 @@
         <f t="shared" si="0"/>
         <v>2883.5439570559997</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3290,8 +3313,9 @@
         <f t="shared" si="0"/>
         <v>74402.301466880002</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -3305,8 +3329,9 @@
         <f t="shared" si="0"/>
         <v>857786.46076908801</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -3320,8 +3345,9 @@
         <f t="shared" si="0"/>
         <v>3599.9898332799999</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -3335,8 +3361,9 @@
         <f t="shared" si="0"/>
         <v>49996.964499647998</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -3350,8 +3377,9 @@
         <f t="shared" si="0"/>
         <v>494055.84498361603</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -3365,8 +3393,9 @@
         <f t="shared" si="0"/>
         <v>137116.71846502399</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -3380,8 +3409,9 @@
         <f t="shared" si="0"/>
         <v>9999.9956789120006</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -3395,8 +3425,9 @@
         <f t="shared" si="0"/>
         <v>399947.62219104002</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -3410,8 +3441,9 @@
         <f t="shared" si="0"/>
         <v>100014.057511744</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -3425,8 +3457,9 @@
         <f t="shared" si="0"/>
         <v>29986.209231424</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -3440,8 +3473,9 @@
         <f t="shared" si="0"/>
         <v>110998.73571404802</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -3455,8 +3489,9 @@
         <f t="shared" si="0"/>
         <v>349919.98054675205</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -3470,8 +3505,9 @@
         <f t="shared" si="0"/>
         <v>20004.619839296</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3485,8 +3521,9 @@
         <f t="shared" si="0"/>
         <v>19999.776079616</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -3500,8 +3537,9 @@
         <f t="shared" si="0"/>
         <v>3996.2093751040002</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -3515,8 +3553,9 @@
         <f t="shared" si="0"/>
         <v>11205.123087296</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -3530,8 +3569,9 @@
         <f t="shared" si="0"/>
         <v>240000.003932992</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -3545,8 +3585,9 @@
         <f t="shared" si="0"/>
         <v>130501.54205049601</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -3560,8 +3601,9 @@
         <f t="shared" si="0"/>
         <v>16002.597952576001</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -3575,8 +3617,9 @@
         <f t="shared" si="0"/>
         <v>499990.41934355197</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -3590,11 +3633,12 @@
         <f t="shared" si="0"/>
         <v>499990.41934355197</v>
       </c>
-      <c r="H26" t="s">
+      <c r="G26" s="2"/>
+      <c r="I26" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -3608,8 +3652,9 @@
         <f t="shared" si="0"/>
         <v>499990.41934355197</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -3619,12 +3664,316 @@
       <c r="F28">
         <v>1</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29">
+        <f>1000512.63*0.000284345</f>
+        <v>284.49076377734997</v>
+      </c>
+      <c r="I29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30">
+        <f>(1028872.44+727611.22+733287.34+56277.3+122055.18+130350.16)*0.000284345</f>
+        <v>795.72630026579998</v>
+      </c>
+      <c r="I30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31">
+        <f>(78241.71+53614.66+65053.12+72956.14+81901.46+70644.79+33603.59)*0.000284345</f>
+        <v>129.66571881714998</v>
+      </c>
+      <c r="I31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+      <c r="I32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="I33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="I34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="I35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="I36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>71</v>
+      </c>
+      <c r="I38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" t="s">
+        <v>71</v>
+      </c>
+      <c r="I39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>71</v>
+      </c>
+      <c r="I40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" t="s">
+        <v>71</v>
+      </c>
+      <c r="I41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" t="s">
+        <v>71</v>
+      </c>
+      <c r="I42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" t="s">
+        <v>71</v>
+      </c>
+      <c r="I43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" t="s">
+        <v>71</v>
+      </c>
+      <c r="I44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" t="s">
+        <v>71</v>
+      </c>
+      <c r="I45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>71</v>
+      </c>
+      <c r="I46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
+      <c r="I47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="I48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" t="s">
+        <v>71</v>
+      </c>
+      <c r="I49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" t="s">
+        <v>71</v>
+      </c>
+      <c r="I50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" t="s">
+        <v>71</v>
+      </c>
+      <c r="I51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
+        <v>71</v>
+      </c>
+      <c r="I52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="I53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" t="s">
+        <v>71</v>
+      </c>
+      <c r="I54" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{48141450-2387-4aca-b41f-19cd6be9dd3c}" enabled="1" method="Standard" siteId="{adf10e2b-b6e9-41d6-be2f-c12bb566019c}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
DMo and Com script update
final updates for CEDARS formatted 8760 output
</commit_message>
<xml_diff>
--- a/scripts/data transformation/Normunits.xlsx
+++ b/scripts/data transformation/Normunits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YLIAN\Documents\DEER_github_2025\DEER-Prototypes-EnergyPlus\scripts\data transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DE9E93-1157-46D4-A64D-6D4477D55686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ED8D93-6437-4E19-9420-262E26D62A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{527A75FC-5BC9-4372-9120-09678A46B600}"/>
   </bookViews>
   <sheets>
     <sheet name="DMo" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="75">
   <si>
     <t>Normunit</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>Com Cap-Ton units for SEER rated AC measures from each com bldg type pre prototype need to be updated</t>
+  </si>
+  <si>
+    <t>SWXX111-00 Example_SEER_AC</t>
   </si>
 </sst>
 </file>
@@ -662,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2593147D-FBCE-4A43-B94C-18CB04EC4F0B}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,7 +748,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -770,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9AEBA2-4873-4E93-88D1-6559970F8CAA}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,7 +844,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -858,7 +861,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -875,7 +878,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -892,7 +895,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -909,7 +912,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -926,7 +929,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -943,7 +946,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -960,7 +963,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -977,7 +980,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -994,7 +997,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -1011,7 +1014,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -1028,7 +1031,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -1045,7 +1048,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -1062,7 +1065,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -1079,7 +1082,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -1096,7 +1099,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -1113,7 +1116,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -1130,7 +1133,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1147,7 +1150,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -1164,7 +1167,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -1181,7 +1184,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
@@ -1198,7 +1201,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -1215,7 +1218,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -1232,7 +1235,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -1249,7 +1252,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
@@ -1266,7 +1269,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
         <v>14</v>
@@ -1283,7 +1286,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
@@ -1300,7 +1303,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
@@ -1317,7 +1320,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
@@ -1334,7 +1337,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
         <v>18</v>
@@ -1351,7 +1354,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
         <v>19</v>
@@ -1368,7 +1371,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
         <v>20</v>
@@ -1400,7 +1403,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
@@ -1417,7 +1420,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -1434,7 +1437,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -1451,7 +1454,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -1468,7 +1471,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
@@ -1485,7 +1488,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
@@ -1502,7 +1505,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
@@ -1519,7 +1522,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
@@ -1536,7 +1539,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
@@ -1553,7 +1556,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
         <v>14</v>
@@ -1570,7 +1573,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B48" t="s">
         <v>15</v>
@@ -1587,7 +1590,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
@@ -1604,7 +1607,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
         <v>17</v>
@@ -1621,7 +1624,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
@@ -1638,7 +1641,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
         <v>19</v>
@@ -1655,7 +1658,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B53" t="s">
         <v>20</v>
@@ -1680,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D254DEF8-D70B-44A9-90B7-19C720405132}">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84:D99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3190,8 +3193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F653D6A-2407-4550-AC1C-A4556A4DAC9A}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32:I54"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3199,7 +3202,8 @@
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="7" width="11.21875" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3675,9 +3679,12 @@
       <c r="C29" t="s">
         <v>71</v>
       </c>
-      <c r="D29">
+      <c r="F29">
         <f>1000512.63*0.000284345</f>
         <v>284.49076377734997</v>
+      </c>
+      <c r="G29" t="s">
+        <v>74</v>
       </c>
       <c r="I29" t="s">
         <v>72</v>
@@ -3690,9 +3697,12 @@
       <c r="C30" t="s">
         <v>71</v>
       </c>
-      <c r="D30">
+      <c r="F30">
         <f>(1028872.44+727611.22+733287.34+56277.3+122055.18+130350.16)*0.000284345</f>
         <v>795.72630026579998</v>
+      </c>
+      <c r="G30" t="s">
+        <v>74</v>
       </c>
       <c r="I30" t="s">
         <v>72</v>
@@ -3705,9 +3715,12 @@
       <c r="C31" t="s">
         <v>71</v>
       </c>
-      <c r="D31">
+      <c r="F31">
         <f>(78241.71+53614.66+65053.12+72956.14+81901.46+70644.79+33603.59)*0.000284345</f>
         <v>129.66571881714998</v>
+      </c>
+      <c r="G31" t="s">
+        <v>74</v>
       </c>
       <c r="I31" t="s">
         <v>72</v>

</xml_diff>